<commit_message>
Update CLIP comparsion and analysis
</commit_message>
<xml_diff>
--- a/vlm/multistage/CLIP comparsion.xlsx
+++ b/vlm/multistage/CLIP comparsion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27716"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\TIL-2024\vlm\yolo-siglip\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\TIL-2024\vlm\multistage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B98A6A9-C363-42EE-8817-7EC7B801946D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC8F265-9BD8-4A90-BC82-6F430C11606D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="2076" windowWidth="17280" windowHeight="9396" xr2:uid="{B8B84376-8849-4309-BD3A-50392A850A58}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B8B84376-8849-4309-BD3A-50392A850A58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="37">
   <si>
     <t>Model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -166,6 +166,30 @@
   </si>
   <si>
     <t>facebook/metaclip-l14-400m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>val before upscale</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>val after upscale (4x lite pad=1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>facebook/metaclip-b32-400m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>openai/clip-vit-large-patch14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>openai/clip-vit-large-patch14-336</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test before upscale</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -190,7 +214,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +233,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -224,24 +260,30 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -253,13 +295,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -596,19 +631,20 @@
   <dimension ref="A1:J97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A92" sqref="A92"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.77734375" customWidth="1"/>
-    <col min="2" max="2" width="31.21875" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="38.5546875" customWidth="1"/>
+    <col min="2" max="2" width="30.21875" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
     <col min="4" max="4" width="17.88671875" customWidth="1"/>
-    <col min="5" max="5" width="30.77734375" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" customWidth="1"/>
-    <col min="7" max="8" width="25.21875" customWidth="1"/>
+    <col min="5" max="5" width="29.88671875" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25.21875" customWidth="1"/>
     <col min="9" max="9" width="11.44140625" customWidth="1"/>
     <col min="10" max="10" width="15.44140625" customWidth="1"/>
   </cols>
@@ -2537,7 +2573,7 @@
       <c r="G62" s="1">
         <v>0.97299999999999998</v>
       </c>
-      <c r="H62" s="2">
+      <c r="H62">
         <v>4</v>
       </c>
       <c r="I62" t="str">
@@ -2571,7 +2607,7 @@
       <c r="G63" s="1">
         <v>0.998</v>
       </c>
-      <c r="H63" s="2">
+      <c r="H63">
         <v>4</v>
       </c>
       <c r="I63" t="str">
@@ -2605,7 +2641,7 @@
       <c r="G64" s="1">
         <v>0.997</v>
       </c>
-      <c r="H64" s="2">
+      <c r="H64">
         <v>4</v>
       </c>
       <c r="I64" t="str">
@@ -2639,7 +2675,7 @@
       <c r="G65" s="1">
         <v>0.999</v>
       </c>
-      <c r="H65" s="2">
+      <c r="H65">
         <v>4</v>
       </c>
       <c r="I65" t="str">
@@ -2673,7 +2709,7 @@
       <c r="G66" s="1">
         <v>1</v>
       </c>
-      <c r="H66" s="2">
+      <c r="H66">
         <v>4</v>
       </c>
       <c r="I66" t="str">
@@ -2707,7 +2743,7 @@
       <c r="G67" s="1">
         <v>0.99199999999999999</v>
       </c>
-      <c r="H67" s="2">
+      <c r="H67">
         <v>4</v>
       </c>
       <c r="I67" t="str">
@@ -2741,7 +2777,7 @@
       <c r="G68" s="1">
         <v>0.98699999999999999</v>
       </c>
-      <c r="H68" s="2">
+      <c r="H68">
         <v>4</v>
       </c>
       <c r="I68" t="str">
@@ -2775,7 +2811,7 @@
       <c r="G69" s="1">
         <v>0.995</v>
       </c>
-      <c r="H69" s="2">
+      <c r="H69">
         <v>4</v>
       </c>
       <c r="I69" t="str">
@@ -2809,7 +2845,7 @@
       <c r="G70" s="1">
         <v>0.997</v>
       </c>
-      <c r="H70" s="2">
+      <c r="H70">
         <v>4</v>
       </c>
       <c r="I70" t="str">
@@ -2843,7 +2879,7 @@
       <c r="G71" s="1">
         <v>0.96799999999999997</v>
       </c>
-      <c r="H71" s="2">
+      <c r="H71">
         <v>4</v>
       </c>
       <c r="I71" t="str">
@@ -2877,7 +2913,7 @@
       <c r="G72" s="1">
         <v>0.98599999999999999</v>
       </c>
-      <c r="H72" s="2">
+      <c r="H72">
         <v>4</v>
       </c>
       <c r="I72" t="str">
@@ -2889,9 +2925,6 @@
         <v>0.98599999999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H73" s="2"/>
-    </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>6</v>
@@ -2914,7 +2947,7 @@
       <c r="G74" s="1">
         <v>0.94199999999999995</v>
       </c>
-      <c r="H74" s="2">
+      <c r="H74">
         <v>4</v>
       </c>
       <c r="I74" t="str">
@@ -2948,7 +2981,7 @@
       <c r="G75" s="1">
         <v>0.99099999999999999</v>
       </c>
-      <c r="H75" s="2">
+      <c r="H75">
         <v>4</v>
       </c>
       <c r="I75" t="str">
@@ -2982,7 +3015,7 @@
       <c r="G76" s="1">
         <v>0.98699999999999999</v>
       </c>
-      <c r="H76" s="2">
+      <c r="H76">
         <v>4</v>
       </c>
       <c r="I76" t="str">
@@ -3016,7 +3049,7 @@
       <c r="G77" s="1">
         <v>0.996</v>
       </c>
-      <c r="H77" s="2">
+      <c r="H77">
         <v>4</v>
       </c>
       <c r="I77" t="str">
@@ -3050,7 +3083,7 @@
       <c r="G78" s="1">
         <v>0.99199999999999999</v>
       </c>
-      <c r="H78" s="2">
+      <c r="H78">
         <v>4</v>
       </c>
       <c r="I78" t="str">
@@ -3084,7 +3117,7 @@
       <c r="G79" s="1">
         <v>0.94</v>
       </c>
-      <c r="H79" s="2">
+      <c r="H79">
         <v>4</v>
       </c>
       <c r="I79" t="str">
@@ -3118,7 +3151,7 @@
       <c r="G80" s="1">
         <v>0.98399999999999999</v>
       </c>
-      <c r="H80" s="2">
+      <c r="H80">
         <v>4</v>
       </c>
       <c r="I80" t="str">
@@ -3152,7 +3185,7 @@
       <c r="G81" s="1">
         <v>0.99099999999999999</v>
       </c>
-      <c r="H81" s="2">
+      <c r="H81">
         <v>4</v>
       </c>
       <c r="I81" t="str">
@@ -3186,7 +3219,7 @@
       <c r="G82" s="1">
         <v>0.99299999999999999</v>
       </c>
-      <c r="H82" s="2">
+      <c r="H82">
         <v>4</v>
       </c>
       <c r="I82" t="str">
@@ -3220,7 +3253,7 @@
       <c r="G83" s="1">
         <v>0.94699999999999995</v>
       </c>
-      <c r="H83" s="2">
+      <c r="H83">
         <v>4</v>
       </c>
       <c r="I83" t="str">
@@ -3254,7 +3287,7 @@
       <c r="G84" s="1">
         <v>0.995</v>
       </c>
-      <c r="H84" s="2">
+      <c r="H84">
         <v>4</v>
       </c>
       <c r="I84" t="str">
@@ -3268,7 +3301,6 @@
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G85" s="1"/>
-      <c r="H85" s="2"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
@@ -3280,9 +3312,18 @@
       <c r="D86" t="s">
         <v>27</v>
       </c>
+      <c r="E86" t="s">
+        <v>31</v>
+      </c>
+      <c r="F86" t="s">
+        <v>32</v>
+      </c>
+      <c r="G86" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
+      <c r="A87" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B87">
@@ -3297,10 +3338,19 @@
         <f>AVERAGE(J14, J50, J74)</f>
         <v>0.61033333333333328</v>
       </c>
+      <c r="E87">
+        <v>0.79873551106427798</v>
+      </c>
+      <c r="F87">
+        <v>0.78205128205128205</v>
+      </c>
+      <c r="G87" s="3">
+        <v>0.66700000000000004</v>
+      </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="3" t="s">
-        <v>7</v>
+      <c r="A88" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="B88">
         <f t="shared" ref="B88:B97" si="2">AVERAGE(J3, J15, J27, J39, J51, J63, J75)</f>
@@ -3314,10 +3364,13 @@
         <f t="shared" ref="D88:D97" si="4">AVERAGE(J15, J51, J75)</f>
         <v>0.92766666666666664</v>
       </c>
+      <c r="E88">
+        <v>0.82033719704952501</v>
+      </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
-        <v>8</v>
+      <c r="A89" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="B89">
         <f t="shared" si="2"/>
@@ -3331,9 +3384,12 @@
         <f t="shared" si="4"/>
         <v>0.95466666666666666</v>
       </c>
+      <c r="E89">
+        <v>0.815946610467158</v>
+      </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="A90" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B90">
@@ -3348,10 +3404,13 @@
         <f t="shared" si="4"/>
         <v>0.99766666666666659</v>
       </c>
+      <c r="E90">
+        <v>0.87671232876712302</v>
+      </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="3" t="s">
-        <v>10</v>
+      <c r="A91" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B91">
         <f t="shared" si="2"/>
@@ -3365,9 +3424,12 @@
         <f t="shared" si="4"/>
         <v>0.94799999999999995</v>
       </c>
+      <c r="E91">
+        <v>0.769582016157358</v>
+      </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="A92" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B92">
@@ -3382,9 +3444,12 @@
         <f t="shared" si="4"/>
         <v>0.96599999999999986</v>
       </c>
+      <c r="E92">
+        <v>0.847383210396909</v>
+      </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="A93" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B93">
@@ -3399,9 +3464,12 @@
         <f t="shared" si="4"/>
         <v>0.95433333333333337</v>
       </c>
+      <c r="E93">
+        <v>0.850895679662803</v>
+      </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="A94" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B94">
@@ -3416,9 +3484,12 @@
         <f t="shared" si="4"/>
         <v>0.98099999999999998</v>
       </c>
+      <c r="E94">
+        <v>0.86406743940990505</v>
+      </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="A95" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B95">
@@ -3433,9 +3504,12 @@
         <f t="shared" si="4"/>
         <v>0.94466666666666665</v>
       </c>
+      <c r="E95">
+        <v>0.82051282051282004</v>
+      </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" s="3" t="s">
+      <c r="A96" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B96">
@@ -3450,9 +3524,12 @@
         <f t="shared" si="4"/>
         <v>0.90499999999999992</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="3" t="s">
+      <c r="E96">
+        <v>0.77994380049174505</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B97">
@@ -3467,10 +3544,13 @@
         <f t="shared" si="4"/>
         <v>0.86033333333333328</v>
       </c>
+      <c r="E97">
+        <v>0.87390235335440802</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="I1:I1048576 J1">
+  <conditionalFormatting sqref="J1 I1:I1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"N"</formula>
     </cfRule>

</xml_diff>

<commit_message>
CLIP test set eval results
</commit_message>
<xml_diff>
--- a/vlm/multistage/CLIP comparsion.xlsx
+++ b/vlm/multistage/CLIP comparsion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\TIL-2024\vlm\multistage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC8F265-9BD8-4A90-BC82-6F430C11606D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AD738B-CECB-4FCA-8835-675CDF033E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B8B84376-8849-4309-BD3A-50392A850A58}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="38">
   <si>
     <t>Model</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -190,6 +190,10 @@
   </si>
   <si>
     <t>test before upscale</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>google/siglip-so400m-patch14-384</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -260,7 +264,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -268,9 +272,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
@@ -631,8 +632,8 @@
   <dimension ref="A1:J97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C86" sqref="C86"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3324,7 +3325,7 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="B87">
         <f>AVERAGE(J2, J14, J26, J38, J50, J62, J74)</f>
@@ -3344,7 +3345,7 @@
       <c r="F87">
         <v>0.78205128205128205</v>
       </c>
-      <c r="G87" s="3">
+      <c r="G87">
         <v>0.66700000000000004</v>
       </c>
     </row>
@@ -3367,6 +3368,9 @@
       <c r="E88">
         <v>0.82033719704952501</v>
       </c>
+      <c r="G88">
+        <v>0.61699999999999999</v>
+      </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
@@ -3387,9 +3391,12 @@
       <c r="E89">
         <v>0.815946610467158</v>
       </c>
+      <c r="G89">
+        <v>0.60499999999999998</v>
+      </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="4" t="s">
+      <c r="A90" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B90">
@@ -3407,6 +3414,9 @@
       <c r="E90">
         <v>0.87671232876712302</v>
       </c>
+      <c r="G90">
+        <v>0.65800000000000003</v>
+      </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
@@ -3429,7 +3439,7 @@
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
+      <c r="A92" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B92">
@@ -3447,9 +3457,12 @@
       <c r="E92">
         <v>0.847383210396909</v>
       </c>
+      <c r="G92">
+        <v>0.63500000000000001</v>
+      </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="5" t="s">
+      <c r="A93" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B93">
@@ -3467,9 +3480,12 @@
       <c r="E93">
         <v>0.850895679662803</v>
       </c>
+      <c r="G93">
+        <v>0.63100000000000001</v>
+      </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
+      <c r="A94" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B94">
@@ -3487,6 +3503,9 @@
       <c r="E94">
         <v>0.86406743940990505</v>
       </c>
+      <c r="G94">
+        <v>0.65800000000000003</v>
+      </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
@@ -3528,8 +3547,8 @@
         <v>0.77994380049174505</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="4" t="s">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B97">
@@ -3546,6 +3565,9 @@
       </c>
       <c r="E97">
         <v>0.87390235335440802</v>
+      </c>
+      <c r="G97">
+        <v>0.64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>